<commit_message>
Updated report and small cleanup of code
</commit_message>
<xml_diff>
--- a/report/result.xlsx
+++ b/report/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Packet Length</t>
   </si>
@@ -293,25 +293,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.4700000000000002</c:v>
+                  <c:v>5.2808000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7429999999999999</c:v>
+                  <c:v>10.249800000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2491999999999996</c:v>
+                  <c:v>12.3996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3885999999999994</c:v>
+                  <c:v>21.824800000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.5974000000000004</c:v>
+                  <c:v>43.9452</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6050000000000004</c:v>
+                  <c:v>61.846400000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.491199999999999</c:v>
+                  <c:v>78.766199999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -834,25 +834,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42109.575000199999</c:v>
+                  <c:v>12056.560546799999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35449.984375</c:v>
+                  <c:v>6512.7465819999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26922.316796600004</c:v>
+                  <c:v>5167.4509766000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17874.0664062</c:v>
+                  <c:v>3192.2816652000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11271.305468800001</c:v>
+                  <c:v>1512.9674315999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6959.0065430000004</c:v>
+                  <c:v>1015.3541750000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3233.7628906</c:v>
+                  <c:v>823.73498519999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1372,25 +1372,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0550000000000002</c:v>
+                  <c:v>7.4378000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9276000000000002</c:v>
+                  <c:v>9.2593999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89919999999999989</c:v>
+                  <c:v>10.157400000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0249999999999999</c:v>
+                  <c:v>10.9292</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4732000000000001</c:v>
+                  <c:v>24.723200000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9010000000000002</c:v>
+                  <c:v>31.4954</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0413999999999994</c:v>
+                  <c:v>79.293400000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1910,25 +1910,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>59604.5273438</c:v>
+                  <c:v>9528.9072265999985</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65810.067968399992</c:v>
+                  <c:v>7267.8867188000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66889.049218800006</c:v>
+                  <c:v>6274.6965820000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59932.048437400001</c:v>
+                  <c:v>5889.7316406</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41435.632031200003</c:v>
+                  <c:v>2661.4764403999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32452.6347656</c:v>
+                  <c:v>2053.4412107999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14886.825586000001</c:v>
+                  <c:v>791.90506559999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4861,22 +4861,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K15"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4886,779 +4887,789 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10000</v>
       </c>
       <c r="B2">
-        <v>1.659</v>
+        <v>5.4660000000000002</v>
       </c>
       <c r="C2">
-        <v>36041.589844000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11319.612305000001</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>1.0900000000000001</v>
+        <v>4.3449999999999998</v>
       </c>
       <c r="C3">
-        <v>54855.960937999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14240.046875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10000</v>
       </c>
       <c r="B4">
-        <v>1.6639999999999999</v>
+        <v>6.6749999999999998</v>
       </c>
       <c r="C4">
-        <v>35933.292969000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9269.3632809999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10000</v>
       </c>
       <c r="B5">
-        <v>1.226</v>
+        <v>5.6539999999999999</v>
       </c>
       <c r="C5">
-        <v>48770.800780999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10943.226562</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10000</v>
       </c>
       <c r="B6">
-        <v>1.7110000000000001</v>
+        <v>4.2640000000000002</v>
       </c>
       <c r="C6">
-        <v>34946.230469000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14510.553711</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5000</v>
       </c>
       <c r="B7">
-        <v>1.46</v>
+        <v>11.090999999999999</v>
       </c>
       <c r="C7">
-        <v>40954.109375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5578.6674800000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5000</v>
       </c>
       <c r="B8">
-        <v>1.603</v>
+        <v>9.3230000000000004</v>
       </c>
       <c r="C8">
-        <v>37300.683594000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6636.5976559999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5000</v>
       </c>
       <c r="B9">
-        <v>1.583</v>
+        <v>9.9770000000000003</v>
       </c>
       <c r="C9">
-        <v>37771.953125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6201.5634769999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5000</v>
       </c>
       <c r="B10">
-        <v>1.6279999999999999</v>
+        <v>6.2409999999999997</v>
       </c>
       <c r="C10">
-        <v>36727.886719000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9913.9560550000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5000</v>
       </c>
       <c r="B11">
-        <v>2.4409999999999998</v>
+        <v>14.617000000000001</v>
       </c>
       <c r="C11">
-        <v>24495.289062</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4232.9482420000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2000</v>
       </c>
       <c r="B12">
-        <v>1.8979999999999999</v>
+        <v>15.391999999999999</v>
       </c>
       <c r="C12">
-        <v>31503.162109000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4019.8154300000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2000</v>
       </c>
       <c r="B13">
-        <v>2.4700000000000002</v>
+        <v>13.548</v>
       </c>
       <c r="C13">
-        <v>24207.691406000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4566.9472660000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2000</v>
       </c>
       <c r="B14">
-        <v>2.016</v>
+        <v>10.211</v>
       </c>
       <c r="C14">
-        <v>29659.226562</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6059.4453119999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2000</v>
       </c>
       <c r="B15">
-        <v>2.508</v>
+        <v>13.468</v>
       </c>
       <c r="C15">
-        <v>23840.910156000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4594.0747069999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2000</v>
       </c>
       <c r="B16">
-        <v>2.3540000000000001</v>
+        <v>9.3789999999999996</v>
       </c>
       <c r="C16">
-        <v>25400.59375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6596.9721680000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1000</v>
       </c>
       <c r="B17">
-        <v>3.6389999999999998</v>
+        <v>27.783999999999999</v>
       </c>
       <c r="C17">
-        <v>16431.162109000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2226.9291990000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1000</v>
       </c>
       <c r="B18">
-        <v>4.0549999999999997</v>
+        <v>30.544</v>
       </c>
       <c r="C18">
-        <v>14745.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2025.700562</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1000</v>
       </c>
       <c r="B19">
-        <v>3.1339999999999999</v>
+        <v>19.161000000000001</v>
       </c>
       <c r="C19">
-        <v>19078.8125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3229.111328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1000</v>
       </c>
       <c r="B20">
-        <v>3.0329999999999999</v>
+        <v>20.218</v>
       </c>
       <c r="C20">
-        <v>19714.144531000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3060.2927249999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1000</v>
       </c>
       <c r="B21">
-        <v>3.0819999999999999</v>
+        <v>11.417</v>
       </c>
       <c r="C21">
-        <v>19400.712890999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5419.3745120000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>500</v>
       </c>
       <c r="B22">
-        <v>4.827</v>
+        <v>56.765000000000001</v>
       </c>
       <c r="C22">
-        <v>12387.196289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1089.9849850000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>500</v>
       </c>
       <c r="B23">
-        <v>4.4219999999999997</v>
+        <v>30.474</v>
       </c>
       <c r="C23">
-        <v>13521.709961</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2030.353638</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>500</v>
       </c>
       <c r="B24">
-        <v>4.875</v>
+        <v>57.524000000000001</v>
       </c>
       <c r="C24">
-        <v>12265.230469</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1075.6032709999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>500</v>
       </c>
       <c r="B25">
-        <v>5.3639999999999999</v>
+        <v>42.781999999999996</v>
       </c>
       <c r="C25">
-        <v>11147.091796999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1446.239014</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>500</v>
       </c>
       <c r="B26">
-        <v>8.4990000000000006</v>
+        <v>32.180999999999997</v>
       </c>
       <c r="C26">
-        <v>7035.298828</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1922.65625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>250</v>
       </c>
       <c r="B27">
-        <v>8.6379999999999999</v>
+        <v>54.692999999999998</v>
       </c>
       <c r="C27">
-        <v>6922.0888670000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1131.278198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>250</v>
       </c>
       <c r="B28">
-        <v>8.5069999999999997</v>
+        <v>53.429000000000002</v>
       </c>
       <c r="C28">
-        <v>7028.6821289999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1158.041504</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>250</v>
       </c>
       <c r="B29">
-        <v>8.4090000000000007</v>
+        <v>71.92</v>
       </c>
       <c r="C29">
-        <v>7110.5952150000003</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>860.30316200000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>250</v>
       </c>
       <c r="B30">
-        <v>9.23</v>
+        <v>59.621000000000002</v>
       </c>
       <c r="C30">
-        <v>6478.1152339999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1037.7719729999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>250</v>
       </c>
       <c r="B31">
-        <v>8.2409999999999997</v>
+        <v>69.569000000000003</v>
       </c>
       <c r="C31">
-        <v>7255.5512699999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>889.37603799999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>100</v>
       </c>
       <c r="B32">
-        <v>18.463999999999999</v>
+        <v>85.817999999999998</v>
       </c>
       <c r="C32">
-        <v>3238.3557129999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>720.97924799999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>100</v>
       </c>
       <c r="B33">
-        <v>18.367000000000001</v>
+        <v>85.572999999999993</v>
       </c>
       <c r="C33">
-        <v>3255.4580080000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>723.04351799999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>100</v>
       </c>
       <c r="B34">
-        <v>18.670999999999999</v>
+        <v>82.635000000000005</v>
       </c>
       <c r="C34">
-        <v>3202.453125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>748.75048800000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>100</v>
       </c>
       <c r="B35">
-        <v>18.620999999999999</v>
+        <v>50.030999999999999</v>
       </c>
       <c r="C35">
-        <v>3211.0520019999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1236.693237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>100</v>
       </c>
       <c r="B36">
-        <v>18.332999999999998</v>
+        <v>89.774000000000001</v>
       </c>
       <c r="C36">
-        <v>3261.4956050000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>689.20843500000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>10000</v>
       </c>
       <c r="B39">
-        <v>0.84399999999999997</v>
+        <v>4.766</v>
       </c>
       <c r="C39">
-        <v>70844.789061999996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12982.166015999999</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>10000</v>
       </c>
       <c r="B40">
-        <v>1.052</v>
+        <v>6.3369999999999997</v>
       </c>
       <c r="C40">
-        <v>56837.449219000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9763.7685550000006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>10000</v>
       </c>
       <c r="B41">
-        <v>0.85</v>
+        <v>5.71</v>
       </c>
       <c r="C41">
-        <v>70344.703125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10835.901367</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10000</v>
       </c>
       <c r="B42">
-        <v>0.97</v>
+        <v>6.4269999999999996</v>
       </c>
       <c r="C42">
-        <v>61642.265625</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9627.0419920000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>10000</v>
       </c>
       <c r="B43">
-        <v>1.5589999999999999</v>
+        <v>13.949</v>
       </c>
       <c r="C43">
-        <v>38353.429687999997</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4435.658203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5000</v>
       </c>
       <c r="B44">
-        <v>0.79500000000000004</v>
+        <v>11.484999999999999</v>
       </c>
       <c r="C44">
-        <v>75211.320311999996</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5387.2880859999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>5000</v>
       </c>
       <c r="B45">
-        <v>0.90900000000000003</v>
+        <v>8.0890000000000004</v>
       </c>
       <c r="C45">
-        <v>65778.882811999996</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7649.0297849999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>5000</v>
       </c>
       <c r="B46">
-        <v>0.77700000000000002</v>
+        <v>7.9480000000000004</v>
       </c>
       <c r="C46">
-        <v>76953.664061999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7784.7255859999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>5000</v>
       </c>
       <c r="B47">
-        <v>1.127</v>
+        <v>13.03</v>
       </c>
       <c r="C47">
-        <v>53055.015625</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4748.5034180000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>5000</v>
       </c>
       <c r="B48">
-        <v>1.03</v>
+        <v>5.7450000000000001</v>
       </c>
       <c r="C48">
-        <v>58051.457030999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10769.886719</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2000</v>
       </c>
       <c r="B49">
-        <v>0.94499999999999995</v>
+        <v>8.41</v>
       </c>
       <c r="C49">
-        <v>63273.015625</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7357.0751950000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2000</v>
       </c>
       <c r="B50">
-        <v>0.97799999999999998</v>
+        <v>13.909000000000001</v>
       </c>
       <c r="C50">
-        <v>61138.039062000003</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4448.4145509999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2000</v>
       </c>
       <c r="B51">
-        <v>0.78400000000000003</v>
+        <v>9.66</v>
       </c>
       <c r="C51">
-        <v>76266.585938000004</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6405.0727539999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>2000</v>
       </c>
       <c r="B52">
-        <v>0.91600000000000004</v>
+        <v>9.5690000000000008</v>
       </c>
       <c r="C52">
-        <v>65276.199219000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6465.9838870000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>2000</v>
       </c>
       <c r="B53">
-        <v>0.873</v>
+        <v>9.2390000000000008</v>
       </c>
       <c r="C53">
-        <v>68491.40625</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6696.9365230000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1000</v>
       </c>
       <c r="B54">
-        <v>1.361</v>
+        <v>8.1630000000000003</v>
       </c>
       <c r="C54">
-        <v>43933.140625</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7579.6889650000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1000</v>
       </c>
       <c r="B55">
-        <v>0.82399999999999995</v>
+        <v>14.477</v>
       </c>
       <c r="C55">
-        <v>72564.320311999996</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4273.8828119999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1000</v>
       </c>
       <c r="B56">
-        <v>0.98199999999999998</v>
+        <v>9.1910000000000007</v>
       </c>
       <c r="C56">
-        <v>60889.003905999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6731.9116210000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1000</v>
       </c>
       <c r="B57">
-        <v>0.94799999999999995</v>
+        <v>10.978</v>
       </c>
       <c r="C57">
-        <v>63072.785155999998</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5636.0903319999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1000</v>
       </c>
       <c r="B58">
-        <v>1.01</v>
+        <v>11.837</v>
       </c>
       <c r="C58">
-        <v>59200.992187999997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5227.0844729999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>500</v>
       </c>
       <c r="B59">
-        <v>1.5640000000000001</v>
+        <v>24.789000000000001</v>
       </c>
       <c r="C59">
-        <v>38230.816405999998</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2495.9860840000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>500</v>
       </c>
       <c r="B60">
-        <v>1.121</v>
+        <v>19.111000000000001</v>
       </c>
       <c r="C60">
-        <v>53338.980469000002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3237.5595699999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>500</v>
       </c>
       <c r="B61">
-        <v>1.5269999999999999</v>
+        <v>32.555</v>
       </c>
       <c r="C61">
-        <v>39157.171875</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1900.568237</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>500</v>
       </c>
       <c r="B62">
-        <v>1.4350000000000001</v>
+        <v>17.123000000000001</v>
       </c>
       <c r="C62">
-        <v>41667.597655999998</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3613.4440920000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>500</v>
       </c>
       <c r="B63">
-        <v>1.7190000000000001</v>
+        <v>30.038</v>
       </c>
       <c r="C63">
-        <v>34783.59375</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2059.8242190000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>250</v>
       </c>
       <c r="B64">
-        <v>1.9830000000000001</v>
+        <v>40.314999999999998</v>
       </c>
       <c r="C64">
-        <v>30152.798827999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1534.739014</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>250</v>
       </c>
       <c r="B65">
-        <v>1.6870000000000001</v>
+        <v>22.111999999999998</v>
       </c>
       <c r="C65">
-        <v>35443.390625</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2798.1640619999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>250</v>
       </c>
       <c r="B66">
-        <v>1.9179999999999999</v>
+        <v>34.454999999999998</v>
       </c>
       <c r="C66">
-        <v>31174.662109000001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1795.7624510000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>250</v>
       </c>
       <c r="B67">
-        <v>2.468</v>
+        <v>26.831</v>
       </c>
       <c r="C67">
-        <v>24227.310547000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2306.0266109999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>250</v>
       </c>
       <c r="B68">
-        <v>1.4490000000000001</v>
+        <v>33.764000000000003</v>
       </c>
       <c r="C68">
-        <v>41265.011719000002</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1832.5139160000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>100</v>
       </c>
       <c r="B69">
-        <v>4.4820000000000002</v>
+        <v>79.266999999999996</v>
       </c>
       <c r="C69">
-        <v>13340.696289</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>915.95849599999997</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>100</v>
       </c>
       <c r="B70">
-        <v>4.3460000000000001</v>
+        <v>89.573999999999998</v>
       </c>
       <c r="C70">
-        <v>13758.167969</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>887.53894000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>100</v>
       </c>
       <c r="B71">
-        <v>3.9489999999999998</v>
+        <v>90.363</v>
       </c>
       <c r="C71">
-        <v>15141.301758</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>684.71612500000003</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>100</v>
       </c>
       <c r="B72">
-        <v>3.7559999999999998</v>
+        <v>69.712999999999994</v>
       </c>
       <c r="C72">
-        <v>15919.329102</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>690.74731399999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>100</v>
       </c>
       <c r="B73">
-        <v>3.6739999999999999</v>
+        <v>67.55</v>
       </c>
       <c r="C73">
-        <v>16274.632812</v>
+        <v>780.56445299999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5666,19 +5677,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC2D2B9-AD20-4B93-AB33-8FB45549299E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="52" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -5692,7 +5703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5701,92 +5712,92 @@
       </c>
       <c r="C2">
         <f>((Sheet1!B2+Sheet1!B3+Sheet1!B4+Sheet1!B5+Sheet1!B6)/5)</f>
-        <v>1.4700000000000002</v>
+        <v>5.2808000000000002</v>
       </c>
       <c r="D2">
         <f>((Sheet1!C2+Sheet1!C3+Sheet1!C4+Sheet1!C5+Sheet1!C6)/5)</f>
-        <v>42109.575000199999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12056.560546799999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>5000</v>
       </c>
       <c r="C3">
         <f>((Sheet1!B7+Sheet1!B8+Sheet1!B9+Sheet1!B10+Sheet1!B11)/5)</f>
-        <v>1.7429999999999999</v>
+        <v>10.249800000000002</v>
       </c>
       <c r="D3">
         <f>((Sheet1!C7+Sheet1!C8+Sheet1!C9+Sheet1!C10+Sheet1!C11)/5)</f>
-        <v>35449.984375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6512.7465819999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4">
         <f>((Sheet1!B12+Sheet1!B13+Sheet1!B14+Sheet1!B15+Sheet1!B16)/5)</f>
-        <v>2.2491999999999996</v>
+        <v>12.3996</v>
       </c>
       <c r="D4">
         <f>((Sheet1!C12+Sheet1!C13+Sheet1!C14+Sheet1!C15+Sheet1!C16)/5)</f>
-        <v>26922.316796600004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5167.4509766000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1000</v>
       </c>
       <c r="C5">
         <f>((Sheet1!B17+Sheet1!B18+Sheet1!B19+Sheet1!B20+Sheet1!B21)/5)</f>
-        <v>3.3885999999999994</v>
+        <v>21.824800000000003</v>
       </c>
       <c r="D5">
         <f>((Sheet1!C17+Sheet1!C18+Sheet1!C19+Sheet1!C20+Sheet1!C21)/5)</f>
-        <v>17874.0664062</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3192.2816652000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>500</v>
       </c>
       <c r="C6">
         <f>((Sheet1!B22+Sheet1!B23+Sheet1!B24+Sheet1!B25+Sheet1!B26)/5)</f>
-        <v>5.5974000000000004</v>
+        <v>43.9452</v>
       </c>
       <c r="D6">
         <f>((Sheet1!C22+Sheet1!C23+Sheet1!C24+Sheet1!C25+Sheet1!C26)/5)</f>
-        <v>11271.305468800001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1512.9674315999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>250</v>
       </c>
       <c r="C7">
         <f>((Sheet1!B27+Sheet1!B28+Sheet1!B29+Sheet1!B30+Sheet1!B31)/5)</f>
-        <v>8.6050000000000004</v>
+        <v>61.846400000000003</v>
       </c>
       <c r="D7">
         <f>((Sheet1!C27+Sheet1!C28+Sheet1!C29+Sheet1!C30+Sheet1!C31)/5)</f>
-        <v>6959.0065430000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1015.3541750000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>100</v>
       </c>
       <c r="C8">
         <f>((Sheet1!B32+Sheet1!B33+Sheet1!B34+Sheet1!B35+Sheet1!B36)/5)</f>
-        <v>18.491199999999999</v>
+        <v>78.766199999999998</v>
       </c>
       <c r="D8">
         <f>((Sheet1!C32+Sheet1!C33+Sheet1!C34+Sheet1!C35+Sheet1!C36)/5)</f>
-        <v>3233.7628906</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>823.73498519999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -5800,7 +5811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -5809,89 +5820,89 @@
       </c>
       <c r="C13">
         <f>((Sheet1!B39+Sheet1!B40+Sheet1!B41+Sheet1!B42+Sheet1!B43)/5)</f>
-        <v>1.0550000000000002</v>
+        <v>7.4378000000000002</v>
       </c>
       <c r="D13">
         <f>((Sheet1!C39+Sheet1!C40+Sheet1!C41+Sheet1!C42+Sheet1!C43)/5)</f>
-        <v>59604.5273438</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9528.9072265999985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>5000</v>
       </c>
       <c r="C14">
         <f>((Sheet1!B44+Sheet1!B45+Sheet1!B46+Sheet1!B47+Sheet1!B48)/5)</f>
-        <v>0.9276000000000002</v>
+        <v>9.2593999999999994</v>
       </c>
       <c r="D14">
         <f>((Sheet1!C44+Sheet1!C45+Sheet1!C46+Sheet1!C47+Sheet1!C48)/5)</f>
-        <v>65810.067968399992</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7267.8867188000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2000</v>
       </c>
       <c r="C15">
         <f>((Sheet1!B49+Sheet1!B50+Sheet1!B51+Sheet1!B52+Sheet1!B53)/5)</f>
-        <v>0.89919999999999989</v>
+        <v>10.157400000000001</v>
       </c>
       <c r="D15">
         <f>((Sheet1!C49+Sheet1!C50+Sheet1!C51+Sheet1!C52+Sheet1!C53)/5)</f>
-        <v>66889.049218800006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6274.6965820000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>1000</v>
       </c>
       <c r="C16">
         <f>((Sheet1!B54+Sheet1!B55+Sheet1!B56+Sheet1!B57+Sheet1!B58)/5)</f>
-        <v>1.0249999999999999</v>
+        <v>10.9292</v>
       </c>
       <c r="D16">
         <f>((Sheet1!C54+Sheet1!C55+Sheet1!C56+Sheet1!C57+Sheet1!C58)/5)</f>
-        <v>59932.048437400001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>5889.7316406</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>500</v>
       </c>
       <c r="C17">
         <f>((Sheet1!B59+Sheet1!B60+Sheet1!B61+Sheet1!B62+Sheet1!B63)/5)</f>
-        <v>1.4732000000000001</v>
+        <v>24.723200000000002</v>
       </c>
       <c r="D17">
         <f>((Sheet1!C59+Sheet1!C60+Sheet1!C61+Sheet1!C62+Sheet1!C63)/5)</f>
-        <v>41435.632031200003</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2661.4764403999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>250</v>
       </c>
       <c r="C18">
         <f>((Sheet1!B64+Sheet1!B65+Sheet1!B66+Sheet1!B67+Sheet1!B68)/5)</f>
-        <v>1.9010000000000002</v>
+        <v>31.4954</v>
       </c>
       <c r="D18">
         <f>((Sheet1!C64+Sheet1!C65+Sheet1!C66+Sheet1!C67+Sheet1!C68)/5)</f>
-        <v>32452.6347656</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2053.4412107999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>100</v>
       </c>
       <c r="C19">
         <f>((Sheet1!B69+Sheet1!B70+Sheet1!B71+Sheet1!B72+Sheet1!B73)/5)</f>
-        <v>4.0413999999999994</v>
+        <v>79.293400000000005</v>
       </c>
       <c r="D19">
         <f>((Sheet1!C69+Sheet1!C70+Sheet1!C71+Sheet1!C72+Sheet1!C73)/5)</f>
-        <v>14886.825586000001</v>
+        <v>791.90506559999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>